<commit_message>
2nd Mock test design completed
</commit_message>
<xml_diff>
--- a/Content/Sample/QuestionFormat_Sample.xlsx
+++ b/Content/Sample/QuestionFormat_Sample.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Dropdown" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -133,9 +132,6 @@
     <t>dd</t>
   </si>
   <si>
-    <t>sdfgvhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjsdfgvsdfgvhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjsdfgvhbsdfgvhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghj</t>
-  </si>
-  <si>
     <t>ABBSBSB</t>
   </si>
   <si>
@@ -152,6 +148,21 @@
   </si>
   <si>
     <t>asdfvasdv</t>
+  </si>
+  <si>
+    <t>sdfgvhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhg ytfrgyhjkhgyfttghjsdf gvs dfgvhbnkj mljhgfdf cvghbnkm,lmjhgfdgvhbnjmkljhgftrdf ghjkml,jhgytfrgyhjkhgyfttghjhbn kjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjsdfgvhbsdfgvhbn kjmljhgfd fcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjnkjmljhgfdfcvghbnkm,lmjhgfdgvh bnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghj</t>
+  </si>
+  <si>
+    <t>sdfgvhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyft t ghjs dfgvsdfgvhbnkjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjk ml,jhgytfrgyhjkhgyfttghjhbnkjmljh gfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjsdfgvhbsdfgvhbnk jmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghjn kjmljhgfdfcvghbnkm,lmjhgfdgvhbnjmkljhgftrdfghjkml,jhgytfrgyhjkhgyfttghj</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Directions (5-8): Read the following passage and answer the questions that follow it. Some words are highlighted to help you to answer some of the questions.</t>
+  </si>
+  <si>
+    <t>Directions (1-4): Read the following passage and answer the questions that follow it. Some words are highlighted to help you to answer some of the questions.</t>
   </si>
 </sst>
 </file>
@@ -199,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
@@ -209,6 +220,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,363 +511,374 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="61" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>7</v>
       </c>
-      <c r="N3" t="s">
-        <v>21</v>
-      </c>
       <c r="P3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
       <c r="P4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>30</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>6</v>
       </c>
-      <c r="N5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>17</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>6</v>
       </c>
-      <c r="N6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="P6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" t="s">
         <v>7</v>
       </c>
-      <c r="N7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
       <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>25</v>
       </c>
-      <c r="J8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" t="s">
         <v>8</v>
       </c>
-      <c r="N8" t="s">
-        <v>33</v>
-      </c>
       <c r="P8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" t="s">
         <v>29</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>6</v>
       </c>
-      <c r="N9" t="s">
-        <v>33</v>
-      </c>
       <c r="P9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Modification and excel sheet added type
</commit_message>
<xml_diff>
--- a/Content/Sample/QuestionFormat_Sample.xlsx
+++ b/Content/Sample/QuestionFormat_Sample.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
   <si>
     <t>Question</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Directions (1-4): Read the following passage and answer the questions that follow it. Some words are highlighted to help you to answer some of the questions.</t>
+  </si>
+  <si>
+    <t>Question Type</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +527,13 @@
     <col min="3" max="3" width="61" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" customWidth="1"/>
     <col min="17" max="17" width="26.85546875" customWidth="1"/>
+    <col min="18" max="18" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -582,8 +585,11 @@
       <c r="Q1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,7 +630,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -659,7 +665,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -694,7 +700,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -726,7 +732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -770,7 +776,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -805,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -843,7 +849,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -882,6 +888,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Correct Answer" prompt="Select Correct Answer from the dropdown" sqref="O1:O1048576">
+      <formula1>"AnswerOption1,AnswerOption2,AnswerOption3,AnswerOption4,AnswerOption5,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the dropdown" sqref="R1:R1048576">
+      <formula1>"Question with description-WITHD, Question without description-WITHOUTD"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Question option 1 mandatory removed
</commit_message>
<xml_diff>
--- a/Content/Sample/QuestionFormat_Sample.xlsx
+++ b/Content/Sample/QuestionFormat_Sample.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
   <si>
     <t>Question</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Question Type</t>
+  </si>
+  <si>
+    <t>Question with description-WITHD</t>
   </si>
 </sst>
 </file>
@@ -552,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="J3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +585,7 @@
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -665,6 +668,9 @@
       <c r="Q2" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="R2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -700,6 +706,9 @@
       <c r="P3" t="s">
         <v>36</v>
       </c>
+      <c r="R3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -735,6 +744,9 @@
       <c r="P4" t="s">
         <v>37</v>
       </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -767,6 +779,9 @@
       <c r="O5" t="s">
         <v>6</v>
       </c>
+      <c r="R5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -811,6 +826,9 @@
       <c r="Q6" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="R6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -846,6 +864,9 @@
       <c r="O7" t="s">
         <v>7</v>
       </c>
+      <c r="R7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -884,6 +905,9 @@
       <c r="P8" t="s">
         <v>39</v>
       </c>
+      <c r="R8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -921,6 +945,9 @@
       </c>
       <c r="P9" t="s">
         <v>40</v>
+      </c>
+      <c r="R9" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>